<commit_message>
Auth commit + db creation
</commit_message>
<xml_diff>
--- a/results/last_result.xlsx
+++ b/results/last_result.xlsx
@@ -463,15 +463,15 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Учитель истории и обществознания</t>
+          <t>Администратор, менеджер по подбору персонала, рекрутер, помощник руководителя</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Вологодская область, г Вологда</t>
+          <t>Томская область, г Томск</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -480,72 +480,72 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>15000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Теории и технологии профессиональной деятельности учителя методиста (Демография)</t>
+          <t>учитель русского языка, учитель английского языка</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Кемеровская область - Кузбасс область, г Новокузнецк</t>
+          <t>г Москва</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Высшее-бакалавриат</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>15000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Учитель истории и обществознания</t>
+          <t>инженер-программист</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Чувашская Республика - чувашия</t>
+          <t>Московская область, г Дубна</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Высшее-бакалавриат</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>20000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Учитель истории и обществознания</t>
+          <t>Педагог, репетитор, администратор, менеджер</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Волгоградская область, г Михайловка</t>
+          <t>Московская область, г Балашиха</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Высшее-бакалавриат</t>
+          <t>Среднее общее</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -555,15 +555,15 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>учитель истории и обществознания</t>
+          <t>менеджер, преподаватель</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Краснодарский край</t>
+          <t>Самарская область, г Самара</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -572,44 +572,44 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>25000</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Педагог, завуч, администратор автоматизированных баз данных, библиограф, библиотекарь, психолог, арт-терапевт</t>
+          <t>Програмист, HTML-верстальщик, Wordpress-разработчик</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Московская область</t>
+          <t>Краснодарский край, г Новороссийск, Натухаевская станица</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Высшее-бакалавриат</t>
+          <t>Среднее общее</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>40000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Преподаватель</t>
+          <t>Педагог-библиотекарь, менеджер научно-исследовательской деятельности, методист, заведующий библиотеки</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Новосибирская область, Купинский район, г Купино</t>
+          <t>Тюменская область, г Тобольск</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -618,21 +618,21 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>35000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Педагог-библиотекарь, менеджер научно-исследовательской деятельности, методист, заведующий библиотеки</t>
+          <t>Программист-экономист, 1с-программист</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Тюменская область, г Тобольск</t>
+          <t>Владимирская область, г Владимир</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -641,21 +641,21 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>25000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>преподаватель истории, русский язык</t>
+          <t>Педагог, завуч, администратор автоматизированных баз данных, библиограф, библиотекарь, психолог, арт-терапевт</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ставропольский край, Минераловодский район, г Минеральные Воды</t>
+          <t>Московская область</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -664,21 +664,21 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>25000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Учитель (преподаватель) русского языка и литературы</t>
+          <t>Педагог-организатор ОБЖ, ОТ и ПБ, ГО и ЧС</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Калужская область, Людиновский район, г. Людиново</t>
+          <t>г Москва</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>18000</v>
+        <v>80000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>